<commit_message>
ReadMe file update and webapplication testcase added in testNG.xml file
</commit_message>
<xml_diff>
--- a/Framework/src/main/java/com/ndtv/resources/TestData.xlsx
+++ b/Framework/src/main/java/com/ndtv/resources/TestData.xlsx
@@ -33,13 +33,13 @@
     <t>APITestData</t>
   </si>
   <si>
-    <t>c</t>
-  </si>
-  <si>
     <t>Allahabad</t>
   </si>
   <si>
     <t>http://api.openweathermap.org/data/2.5/weather</t>
+  </si>
+  <si>
+    <t>7fe67bf08c80ded756e598d6f8fedaea</t>
   </si>
 </sst>
 </file>
@@ -381,7 +381,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -405,13 +405,13 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
         <v>7</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Final Commit :  Updated testcases with logger and added comparator and variance logic getting data from external file and some minor changes to multiple supported classes
</commit_message>
<xml_diff>
--- a/Framework/src/main/java/com/ndtv/resources/TestData.xlsx
+++ b/Framework/src/main/java/com/ndtv/resources/TestData.xlsx
@@ -16,30 +16,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t>BaseURL</t>
-  </si>
-  <si>
-    <t>CityName</t>
-  </si>
-  <si>
-    <t>AccessKey</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>TestCase</t>
   </si>
   <si>
-    <t>APITestData</t>
+    <t>TempVariance</t>
   </si>
   <si>
-    <t>Allahabad</t>
-  </si>
-  <si>
-    <t>http://api.openweathermap.org/data/2.5/weather</t>
-  </si>
-  <si>
-    <t>7fe67bf08c80ded756e598d6f8fedaea</t>
+    <t>Temperature(in Celsius)</t>
   </si>
 </sst>
 </file>
@@ -378,40 +363,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="11.453125" customWidth="1"/>
+    <col min="2" max="2" width="19.6328125" customWidth="1"/>
+    <col min="3" max="3" width="17.7265625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
+      <c r="B2">
+        <v>29.26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>